<commit_message>
Messing with testing frameworks.  Very little success
</commit_message>
<xml_diff>
--- a/doc/baseball_stats.xlsx
+++ b/doc/baseball_stats.xlsx
@@ -488,7 +488,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -585,6 +585,49 @@
     <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>14</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <f>E3+F3*2+G3*3+H3*4</f>
+        <v>13</v>
+      </c>
+      <c r="L3">
+        <f>D3/B3</f>
+        <v>0.625</v>
+      </c>
+      <c r="M3">
+        <f>(D3+J3)/(K3+J3)</f>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="N3">
+        <f>K3/B3</f>
+        <v>1.625</v>
       </c>
     </row>
     <row r="4" spans="1:14">

</xml_diff>